<commit_message>
benchmark now measures the time it takes each file to transmit
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12" xml:space="preserve">
   <si>
-    <t>Time (sec)</t>
+    <t>Avg Time (sec)</t>
   </si>
   <si>
     <t>Packet Loss</t>
@@ -35,10 +35,10 @@
     <t>Local</t>
   </si>
   <si>
-    <t>small.txt (45 Bytes)</t>
-  </si>
-  <si>
-    <t>medium.jpg (44.43 KB)</t>
+    <t>small.txt (45 Bytes) (10 times)</t>
+  </si>
+  <si>
+    <t>medium.jpg (44.43 KB) (10 times)</t>
   </si>
   <si>
     <t>LAN</t>
@@ -136,10 +136,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="9"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="9"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="9"/>
@@ -217,10 +217,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.144768999889493</v>
+        <v>0.0030138000147417188</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.7574269999749959</v>
+        <v>0.002043300005607307</v>
       </c>
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
@@ -235,10 +235,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.990896999835968</v>
+        <v>0.04863890000851825</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.03570100013166666</v>
+        <v>0.0057667999877594415</v>
       </c>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
@@ -254,10 +254,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.7332550000865012</v>
+        <v>0.004543900047428906</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.7387779999990016</v>
+        <v>0.003966900007799268</v>
       </c>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
@@ -272,10 +272,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.5862090000882745</v>
+        <v>0.07063169997418299</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.35154400020837784</v>
+        <v>0.010418599983677269</v>
       </c>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
@@ -291,10 +291,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.27763600018806756</v>
+        <v>0.23238089999649675</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.9136910000815988</v>
+        <v>0.77170329997316</v>
       </c>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
@@ -309,10 +309,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0.4997030000668019</v>
+        <v>0.3117841000203043</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.5889889998361468</v>
+        <v>0.9604642999940551</v>
       </c>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>

</xml_diff>

<commit_message>
added fin command at end of recieve for redundency. added mutex for acks. Better json command parsing
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -41,13 +41,13 @@
     <t>Local</t>
   </si>
   <si>
-    <t>small.txt (45 Bytes) (10 times)</t>
-  </si>
-  <si>
-    <t>medium.jpg (44.43 KB) (10 times)</t>
-  </si>
-  <si>
-    <t>LAN</t>
+    <t>tiny.txt (45 Bytes) (10 times)</t>
+  </si>
+  <si>
+    <t>small.jpg (44.43 KB) (10 times)</t>
+  </si>
+  <si>
+    <t>medium.jpg (2.248 MB) (5 times)</t>
   </si>
   <si>
     <t>Internet</t>
@@ -234,16 +234,16 @@
         <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.004403300000558374</v>
+        <v>0.003003400003944989</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.0023888000017905143</v>
+        <v>0.003274299998884089</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>0.00857350000005681</v>
+        <v>0.006583900001714937</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>-0.7213740010760267</v>
+        <v>-0.5026807822064099</v>
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
@@ -257,116 +257,115 @@
         <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.06377290000018547</v>
+        <v>0.04829529999988154</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.013325999998050975</v>
+        <v>0.009827900004165713</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0.053369599999132336</v>
+        <v>0.04428600000101142</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>-0.7503072910745514</v>
+        <v>-0.7780811090651388</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
       <c r="I4" s="0"/>
     </row>
-    <row r="5"/>
-    <row r="6">
-      <c r="A6" s="0" t="s">
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.005572300001222175</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.0054616999994323125</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>0.011270499999227468</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>-0.5153986069999839</v>
-      </c>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
-      <c r="I6" s="0"/>
-    </row>
+      <c r="C5" s="0" t="n">
+        <v>1.286583599995356</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.7791729999997188</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.5591157999995631</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>0.3935807215613074</v>
+      </c>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+    </row>
+    <row r="6"/>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.0920122999988962</v>
+        <v>0.2364815999972052</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.013059699999575968</v>
+        <v>0.466005099999893</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0.09892850000032923</v>
+        <v>1.2279490999993867</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>-0.8679884967473225</v>
+        <v>-0.6205012895077444</v>
       </c>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
     </row>
-    <row r="8"/>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.3175075000021025</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.950518700000248</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1.3214909000016632</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>-0.2807224779231914</v>
+      </c>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+    </row>
     <row r="9">
       <c r="A9" s="0" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.23611000000018975</v>
+        <v>3.2856530000048223</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.46764579999944544</v>
+        <v>3.828223200002685</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1.1968429999993533</v>
+        <v>4.650853400002234</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v>-0.6092672138286324</v>
+        <v>-0.17687725869818938</v>
       </c>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
     </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>0.3372002000003704</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>0.9493998999983887</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>2.961587999999028</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>-0.6794287726723973</v>
-      </c>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
-    </row>
-    <row r="11"/>
+    <row r="10"/>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
11/implement udt v1 (#12)
* implmeented send

* implemented receive, hopefully

* wrote benchmark for udt

* various bug fixes

* excel pretty ness

* renamed test files and added medium.png

* made some change

* added fin command at end of recieve for redundency. added mutex for acks. Better json command parsing
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -9,11 +9,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14" xml:space="preserve">
   <si>
     <t>Avg Time (sec)</t>
   </si>
   <si>
+    <t>% Faster</t>
+  </si>
+  <si>
     <t>Packet Loss</t>
   </si>
   <si>
@@ -32,16 +35,19 @@
     <t>UDT</t>
   </si>
   <si>
+    <t>Than TCP</t>
+  </si>
+  <si>
     <t>Local</t>
   </si>
   <si>
-    <t>small.txt (45 Bytes) (10 times)</t>
-  </si>
-  <si>
-    <t>medium.jpg (44.43 KB) (10 times)</t>
-  </si>
-  <si>
-    <t>LAN</t>
+    <t>tiny.txt (45 Bytes) (10 times)</t>
+  </si>
+  <si>
+    <t>small.jpg (44.43 KB) (10 times)</t>
+  </si>
+  <si>
+    <t>medium.jpg (2.248 MB) (5 times)</t>
   </si>
   <si>
     <t>Internet</t>
@@ -51,9 +57,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
+    <numFmt numFmtId="102" formatCode="[GREEN]0.00%;-[RED]0.00%"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -104,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
@@ -114,6 +121,9 @@
     </xf>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" numFmtId="102" fontId="0" fillId="0" applyNumberFormat="true" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -140,9 +150,10 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="10"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="10"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="9"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="9"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -172,12 +183,15 @@
       <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -185,22 +199,22 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>5</v>
@@ -208,123 +222,155 @@
       <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.0030138000147417188</v>
+        <v>0.003003400003944989</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.002043300005607307</v>
-      </c>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
+        <v>0.003274299998884089</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.006583900001714937</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>-0.5026807822064099</v>
+      </c>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.04863890000851825</v>
+        <v>0.04829529999988154</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.0057667999877594415</v>
-      </c>
-      <c r="E4" s="0"/>
-      <c r="F4" s="0"/>
+        <v>0.009827900004165713</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.04428600000101142</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>-0.7780811090651388</v>
+      </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
-    </row>
-    <row r="5"/>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.004543900047428906</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.003966900007799268</v>
-      </c>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
-    </row>
+      <c r="I4" s="0"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1.286583599995356</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.7791729999997188</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.5591157999995631</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>0.3935807215613074</v>
+      </c>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+    </row>
+    <row r="6"/>
     <row r="7">
       <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C7" s="0" t="n">
-        <v>0.07063169997418299</v>
+        <v>0.2364815999972052</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.010418599983677269</v>
-      </c>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
+        <v>0.466005099999893</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1.2279490999993867</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>-0.6205012895077444</v>
+      </c>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
-    </row>
-    <row r="8"/>
+      <c r="I7" s="0"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.3175075000021025</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.950518700000248</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1.3214909000016632</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>-0.2807224779231914</v>
+      </c>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+    </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.23238089999649675</v>
+        <v>3.2856530000048223</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.77170329997316</v>
-      </c>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
+        <v>3.828223200002685</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>4.650853400002234</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>-0.17687725869818938</v>
+      </c>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>0.3117841000203043</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>0.9604642999940551</v>
-      </c>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
-    </row>
-    <row r="11"/>
+      <c r="I9" s="0"/>
+    </row>
+    <row r="10"/>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
   <mergeCells count="2">
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>

</xml_diff>